<commit_message>
Added a column for total stack use
</commit_message>
<xml_diff>
--- a/logging/tests-stm8l152c6/atomthreads-test-results.xlsx
+++ b/logging/tests-stm8l152c6/atomthreads-test-results.xlsx
@@ -11,12 +11,12 @@
     <sheet name="Device configuration" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="75">
   <si>
     <t>Test ID</t>
   </si>
@@ -238,6 +238,9 @@
   </si>
   <si>
     <t>sem8</t>
+  </si>
+  <si>
+    <t>TotalUse</t>
   </si>
 </sst>
 </file>
@@ -283,7 +286,11 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="7">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -313,19 +320,22 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:G41" totalsRowShown="0">
-  <autoFilter ref="A1:G41"/>
-  <sortState ref="A2:G41">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:H41" totalsRowShown="0">
+  <autoFilter ref="A1:H41"/>
+  <sortState ref="A2:H41">
     <sortCondition ref="A1:A41"/>
   </sortState>
-  <tableColumns count="7">
+  <tableColumns count="8">
     <tableColumn id="1" name="Test ID"/>
-    <tableColumn id="2" name="StackUse1" dataDxfId="5"/>
-    <tableColumn id="3" name="StackUse2" dataDxfId="4"/>
-    <tableColumn id="6" name="StackUse3" dataDxfId="3"/>
-    <tableColumn id="7" name="StackUse4" dataDxfId="2"/>
-    <tableColumn id="4" name="MainUse" dataDxfId="1"/>
-    <tableColumn id="5" name="Result" dataDxfId="0"/>
+    <tableColumn id="2" name="StackUse1" dataDxfId="6"/>
+    <tableColumn id="3" name="StackUse2" dataDxfId="5"/>
+    <tableColumn id="6" name="StackUse3" dataDxfId="4"/>
+    <tableColumn id="7" name="StackUse4" dataDxfId="3"/>
+    <tableColumn id="4" name="MainUse" dataDxfId="2"/>
+    <tableColumn id="8" name="TotalUse" dataDxfId="0">
+      <calculatedColumnFormula>SUM(Table1[[#This Row],[StackUse1]:[MainUse]])</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" name="Result" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -618,10 +628,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G41"/>
+  <dimension ref="A1:H41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A42" sqref="A42"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -629,11 +639,12 @@
     <col min="1" max="1" width="8.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="5" width="11.88671875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="2.77734375" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" customWidth="1"/>
+    <col min="8" max="8" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="2.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -653,10 +664,13 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -667,11 +681,15 @@
       <c r="F2" s="1">
         <v>124</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G2" s="1">
+        <f>SUM(Table1[[#This Row],[StackUse1]:[MainUse]])</f>
+        <v>124</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -682,11 +700,15 @@
       <c r="F3" s="1">
         <v>124</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G3" s="1">
+        <f>SUM(Table1[[#This Row],[StackUse1]:[MainUse]])</f>
+        <v>124</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>46</v>
       </c>
@@ -701,11 +723,15 @@
       <c r="F4" s="1">
         <v>140</v>
       </c>
-      <c r="G4" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G4" s="1">
+        <f>SUM(Table1[[#This Row],[StackUse1]:[MainUse]])</f>
+        <v>258</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>47</v>
       </c>
@@ -724,11 +750,15 @@
       <c r="F5" s="1">
         <v>148</v>
       </c>
-      <c r="G5" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G5" s="1">
+        <f>SUM(Table1[[#This Row],[StackUse1]:[MainUse]])</f>
+        <v>408</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>42</v>
       </c>
@@ -743,11 +773,15 @@
       <c r="F6" s="1">
         <v>144</v>
       </c>
-      <c r="G6" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G6" s="1">
+        <f>SUM(Table1[[#This Row],[StackUse1]:[MainUse]])</f>
+        <v>246</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>43</v>
       </c>
@@ -760,11 +794,15 @@
       <c r="F7" s="1">
         <v>151</v>
       </c>
-      <c r="G7" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G7" s="1">
+        <f>SUM(Table1[[#This Row],[StackUse1]:[MainUse]])</f>
+        <v>198</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>54</v>
       </c>
@@ -783,11 +821,15 @@
       <c r="F8" s="1">
         <v>140</v>
       </c>
-      <c r="G8" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G8" s="1">
+        <f>SUM(Table1[[#This Row],[StackUse1]:[MainUse]])</f>
+        <v>344</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>55</v>
       </c>
@@ -806,11 +848,15 @@
       <c r="F9" s="1">
         <v>141</v>
       </c>
-      <c r="G9" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G9" s="1">
+        <f>SUM(Table1[[#This Row],[StackUse1]:[MainUse]])</f>
+        <v>470</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>56</v>
       </c>
@@ -823,11 +869,15 @@
       <c r="F10" s="1">
         <v>140</v>
       </c>
-      <c r="G10" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G10" s="1">
+        <f>SUM(Table1[[#This Row],[StackUse1]:[MainUse]])</f>
+        <v>198</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>57</v>
       </c>
@@ -840,11 +890,15 @@
       <c r="F11" s="1">
         <v>140</v>
       </c>
-      <c r="G11" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G11" s="1">
+        <f>SUM(Table1[[#This Row],[StackUse1]:[MainUse]])</f>
+        <v>212</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>58</v>
       </c>
@@ -857,11 +911,15 @@
       <c r="F12" s="1">
         <v>150</v>
       </c>
-      <c r="G12" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G12" s="1">
+        <f>SUM(Table1[[#This Row],[StackUse1]:[MainUse]])</f>
+        <v>197</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>59</v>
       </c>
@@ -878,11 +936,15 @@
       <c r="F13" s="1">
         <v>140</v>
       </c>
-      <c r="G13" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G13" s="1">
+        <f>SUM(Table1[[#This Row],[StackUse1]:[MainUse]])</f>
+        <v>299</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>60</v>
       </c>
@@ -895,11 +957,15 @@
       <c r="F14" s="1">
         <v>148</v>
       </c>
-      <c r="G14" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G14" s="1">
+        <f>SUM(Table1[[#This Row],[StackUse1]:[MainUse]])</f>
+        <v>195</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -910,11 +976,15 @@
       <c r="F15" s="1">
         <v>124</v>
       </c>
-      <c r="G15" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G15" s="1">
+        <f>SUM(Table1[[#This Row],[StackUse1]:[MainUse]])</f>
+        <v>124</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>62</v>
       </c>
@@ -925,11 +995,15 @@
       <c r="F16" s="1">
         <v>124</v>
       </c>
-      <c r="G16" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G16" s="1">
+        <f>SUM(Table1[[#This Row],[StackUse1]:[MainUse]])</f>
+        <v>124</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>41</v>
       </c>
@@ -944,11 +1018,15 @@
       <c r="F17" s="1">
         <v>140</v>
       </c>
-      <c r="G17" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G17" s="1">
+        <f>SUM(Table1[[#This Row],[StackUse1]:[MainUse]])</f>
+        <v>252</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>63</v>
       </c>
@@ -963,11 +1041,15 @@
       <c r="F18" s="1">
         <v>141</v>
       </c>
-      <c r="G18" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G18" s="1">
+        <f>SUM(Table1[[#This Row],[StackUse1]:[MainUse]])</f>
+        <v>253</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>64</v>
       </c>
@@ -978,11 +1060,15 @@
       <c r="F19" s="1">
         <v>124</v>
       </c>
-      <c r="G19" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G19" s="1">
+        <f>SUM(Table1[[#This Row],[StackUse1]:[MainUse]])</f>
+        <v>124</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>65</v>
       </c>
@@ -1001,11 +1087,15 @@
       <c r="F20" s="1">
         <v>141</v>
       </c>
-      <c r="G20" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G20" s="1">
+        <f>SUM(Table1[[#This Row],[StackUse1]:[MainUse]])</f>
+        <v>385</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>66</v>
       </c>
@@ -1018,11 +1108,15 @@
       <c r="F21" s="1">
         <v>146</v>
       </c>
-      <c r="G21" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G21" s="1">
+        <f>SUM(Table1[[#This Row],[StackUse1]:[MainUse]])</f>
+        <v>218</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>67</v>
       </c>
@@ -1039,11 +1133,15 @@
       <c r="F22" s="1">
         <v>140</v>
       </c>
-      <c r="G22" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G22" s="1">
+        <f>SUM(Table1[[#This Row],[StackUse1]:[MainUse]])</f>
+        <v>314</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>68</v>
       </c>
@@ -1054,11 +1152,15 @@
       <c r="F23" s="1">
         <v>124</v>
       </c>
-      <c r="G23" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G23" s="1">
+        <f>SUM(Table1[[#This Row],[StackUse1]:[MainUse]])</f>
+        <v>124</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>69</v>
       </c>
@@ -1077,11 +1179,15 @@
       <c r="F24" s="1">
         <v>141</v>
       </c>
-      <c r="G24" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G24" s="1">
+        <f>SUM(Table1[[#This Row],[StackUse1]:[MainUse]])</f>
+        <v>498</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>1</v>
       </c>
@@ -1096,11 +1202,15 @@
       <c r="F25" s="1">
         <v>149</v>
       </c>
-      <c r="G25" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G25" s="1">
+        <f>SUM(Table1[[#This Row],[StackUse1]:[MainUse]])</f>
+        <v>251</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>7</v>
       </c>
@@ -1111,11 +1221,15 @@
       <c r="F26" s="1">
         <v>124</v>
       </c>
-      <c r="G26" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G26" s="1">
+        <f>SUM(Table1[[#This Row],[StackUse1]:[MainUse]])</f>
+        <v>124</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>8</v>
       </c>
@@ -1134,11 +1248,15 @@
       <c r="F27" s="1">
         <v>140</v>
       </c>
-      <c r="G27" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G27" s="1">
+        <f>SUM(Table1[[#This Row],[StackUse1]:[MainUse]])</f>
+        <v>344</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>11</v>
       </c>
@@ -1157,11 +1275,15 @@
       <c r="F28" s="1">
         <v>139</v>
       </c>
-      <c r="G28" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G28" s="1">
+        <f>SUM(Table1[[#This Row],[StackUse1]:[MainUse]])</f>
+        <v>474</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>70</v>
       </c>
@@ -1174,11 +1296,15 @@
       <c r="F29" s="1">
         <v>140</v>
       </c>
-      <c r="G29" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G29" s="1">
+        <f>SUM(Table1[[#This Row],[StackUse1]:[MainUse]])</f>
+        <v>191</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>71</v>
       </c>
@@ -1191,11 +1317,15 @@
       <c r="F30" s="1">
         <v>140</v>
       </c>
-      <c r="G30" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G30" s="1">
+        <f>SUM(Table1[[#This Row],[StackUse1]:[MainUse]])</f>
+        <v>191</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>72</v>
       </c>
@@ -1208,11 +1338,15 @@
       <c r="F31" s="1">
         <v>140</v>
       </c>
-      <c r="G31" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G31" s="1">
+        <f>SUM(Table1[[#This Row],[StackUse1]:[MainUse]])</f>
+        <v>224</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>73</v>
       </c>
@@ -1229,11 +1363,15 @@
       <c r="F32" s="1">
         <v>154</v>
       </c>
-      <c r="G32" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G32" s="1">
+        <f>SUM(Table1[[#This Row],[StackUse1]:[MainUse]])</f>
+        <v>333</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>61</v>
       </c>
@@ -1250,11 +1388,15 @@
       <c r="F33" s="1">
         <v>140</v>
       </c>
-      <c r="G33" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G33" s="1">
+        <f>SUM(Table1[[#This Row],[StackUse1]:[MainUse]])</f>
+        <v>299</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>44</v>
       </c>
@@ -1265,11 +1407,15 @@
       <c r="F34" s="1">
         <v>124</v>
       </c>
-      <c r="G34" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G34" s="1">
+        <f>SUM(Table1[[#This Row],[StackUse1]:[MainUse]])</f>
+        <v>124</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>45</v>
       </c>
@@ -1286,11 +1432,15 @@
       <c r="F35" s="1">
         <v>140</v>
       </c>
-      <c r="G35" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G35" s="1">
+        <f>SUM(Table1[[#This Row],[StackUse1]:[MainUse]])</f>
+        <v>317</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>48</v>
       </c>
@@ -1301,11 +1451,15 @@
       <c r="F36" s="1">
         <v>124</v>
       </c>
-      <c r="G36" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G36" s="1">
+        <f>SUM(Table1[[#This Row],[StackUse1]:[MainUse]])</f>
+        <v>124</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>49</v>
       </c>
@@ -1316,11 +1470,15 @@
       <c r="F37" s="1">
         <v>124</v>
       </c>
-      <c r="G37" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G37" s="1">
+        <f>SUM(Table1[[#This Row],[StackUse1]:[MainUse]])</f>
+        <v>124</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>50</v>
       </c>
@@ -1331,11 +1489,15 @@
       <c r="F38" s="1">
         <v>124</v>
       </c>
-      <c r="G38" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G38" s="1">
+        <f>SUM(Table1[[#This Row],[StackUse1]:[MainUse]])</f>
+        <v>124</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>51</v>
       </c>
@@ -1346,11 +1508,15 @@
       <c r="F39" s="1">
         <v>124</v>
       </c>
-      <c r="G39" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G39" s="1">
+        <f>SUM(Table1[[#This Row],[StackUse1]:[MainUse]])</f>
+        <v>124</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>52</v>
       </c>
@@ -1361,11 +1527,15 @@
       <c r="F40" s="1">
         <v>124</v>
       </c>
-      <c r="G40" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G40" s="1">
+        <f>SUM(Table1[[#This Row],[StackUse1]:[MainUse]])</f>
+        <v>124</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>53</v>
       </c>
@@ -1376,7 +1546,11 @@
       <c r="F41" s="1">
         <v>124</v>
       </c>
-      <c r="G41" s="1" t="s">
+      <c r="G41" s="1">
+        <f>SUM(Table1[[#This Row],[StackUse1]:[MainUse]])</f>
+        <v>124</v>
+      </c>
+      <c r="H41" s="1" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added descriptions of the type of test to the different tests
</commit_message>
<xml_diff>
--- a/logging/tests-stm8l152c6/atomthreads-test-results.xlsx
+++ b/logging/tests-stm8l152c6/atomthreads-test-results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="245" yWindow="109" windowWidth="14808" windowHeight="8015"/>
   </bookViews>
   <sheets>
     <sheet name="Results" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="112">
   <si>
     <t>Test ID</t>
   </si>
@@ -241,6 +241,117 @@
   </si>
   <si>
     <t>TotalUse</t>
+  </si>
+  <si>
+    <t>Semaphore creation and deletion API</t>
+  </si>
+  <si>
+    <t>atomSemGet() and atomSemPut</t>
+  </si>
+  <si>
+    <t>Semaphore priority and FIFO on waking threads</t>
+  </si>
+  <si>
+    <t>Synchronisation between threads</t>
+  </si>
+  <si>
+    <t>Semaphore stress test Get and Put</t>
+  </si>
+  <si>
+    <t>Semaphore basic counting test</t>
+  </si>
+  <si>
+    <t>Semaphore for basic mutual exclusion test</t>
+  </si>
+  <si>
+    <t>Semaphore deletion API with multiple blocked threads</t>
+  </si>
+  <si>
+    <t>atomTimerDelay() API test</t>
+  </si>
+  <si>
+    <t>atomTimerDelay() with 3 threads test</t>
+  </si>
+  <si>
+    <t>atomTimerRegister() API test</t>
+  </si>
+  <si>
+    <t>atomTimerCancel() API test</t>
+  </si>
+  <si>
+    <t>timer subsystem behaviour test</t>
+  </si>
+  <si>
+    <t>timer register within a timer callback test</t>
+  </si>
+  <si>
+    <t>Basic context-switch test</t>
+  </si>
+  <si>
+    <t>Bad parameter handling of public API test</t>
+  </si>
+  <si>
+    <t>Scheduling with different priorities and preemption test</t>
+  </si>
+  <si>
+    <t>Round-Robin timeslicing test</t>
+  </si>
+  <si>
+    <t>Timeouts on mutex test</t>
+  </si>
+  <si>
+    <t>Mutex creation and deletion API test</t>
+  </si>
+  <si>
+    <t>atomMutexGet() and atomMutexPUT() API test</t>
+  </si>
+  <si>
+    <t>Stress test the mutex Get and Put operations</t>
+  </si>
+  <si>
+    <t>Mutex priority and FIFO on waking threads test</t>
+  </si>
+  <si>
+    <t>Basic mutex usage test</t>
+  </si>
+  <si>
+    <t>Mutex lock count test</t>
+  </si>
+  <si>
+    <t>Mutex ownership test</t>
+  </si>
+  <si>
+    <t>Mutex deletion API test</t>
+  </si>
+  <si>
+    <t>Queue creation and deletion API test</t>
+  </si>
+  <si>
+    <t>Queue deletion while threads blocking on atomQueueGet() test</t>
+  </si>
+  <si>
+    <t>Queue deletion while threads blocking on atomQueuePut() test</t>
+  </si>
+  <si>
+    <t>atomQueueGet() and atomQueuePut() stress test</t>
+  </si>
+  <si>
+    <t>Queue priority and FIFO on waking threads test</t>
+  </si>
+  <si>
+    <t>Queue basic operation test</t>
+  </si>
+  <si>
+    <t>Queue deletion API test</t>
+  </si>
+  <si>
+    <t>Timeout on queue test</t>
+  </si>
+  <si>
+    <t>Queue get and put stress test</t>
+  </si>
+  <si>
+    <t>Test type</t>
   </si>
 </sst>
 </file>
@@ -276,22 +387,28 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="8">
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -320,22 +437,23 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:H41" totalsRowShown="0">
-  <autoFilter ref="A1:H41"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:I41" totalsRowShown="0">
+  <autoFilter ref="A1:I41"/>
   <sortState ref="A2:H41">
     <sortCondition ref="A1:A41"/>
   </sortState>
-  <tableColumns count="8">
+  <tableColumns count="9">
     <tableColumn id="1" name="Test ID"/>
-    <tableColumn id="2" name="StackUse1" dataDxfId="6"/>
-    <tableColumn id="3" name="StackUse2" dataDxfId="5"/>
-    <tableColumn id="6" name="StackUse3" dataDxfId="4"/>
-    <tableColumn id="7" name="StackUse4" dataDxfId="3"/>
-    <tableColumn id="4" name="MainUse" dataDxfId="2"/>
-    <tableColumn id="8" name="TotalUse" dataDxfId="0">
+    <tableColumn id="2" name="StackUse1" dataDxfId="7"/>
+    <tableColumn id="3" name="StackUse2" dataDxfId="6"/>
+    <tableColumn id="6" name="StackUse3" dataDxfId="5"/>
+    <tableColumn id="7" name="StackUse4" dataDxfId="4"/>
+    <tableColumn id="4" name="MainUse" dataDxfId="3"/>
+    <tableColumn id="8" name="TotalUse" dataDxfId="2">
       <calculatedColumnFormula>SUM(Table1[[#This Row],[StackUse1]:[MainUse]])</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" name="Result" dataDxfId="1"/>
+    <tableColumn id="9" name="Test type" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -628,23 +746,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H41"/>
+  <dimension ref="A1:I41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="H41" sqref="H41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.6640625" customWidth="1"/>
-    <col min="8" max="8" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="2.77734375" customWidth="1"/>
+    <col min="1" max="1" width="8.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.625" customWidth="1"/>
+    <col min="8" max="8" width="8.375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="53.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -669,8 +787,11 @@
       <c r="H1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -688,8 +809,11 @@
       <c r="H2" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I2" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -707,8 +831,11 @@
       <c r="H3" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I3" s="3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>46</v>
       </c>
@@ -730,8 +857,11 @@
       <c r="H4" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I4" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>47</v>
       </c>
@@ -757,8 +887,11 @@
       <c r="H5" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I5" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>42</v>
       </c>
@@ -780,8 +913,11 @@
       <c r="H6" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I6" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>43</v>
       </c>
@@ -801,8 +937,11 @@
       <c r="H7" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I7" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>54</v>
       </c>
@@ -828,8 +967,11 @@
       <c r="H8" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I8" s="3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>55</v>
       </c>
@@ -855,8 +997,11 @@
       <c r="H9" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I9" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>56</v>
       </c>
@@ -876,8 +1021,11 @@
       <c r="H10" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I10" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>57</v>
       </c>
@@ -897,8 +1045,11 @@
       <c r="H11" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I11" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>58</v>
       </c>
@@ -918,8 +1069,11 @@
       <c r="H12" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I12" s="3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>59</v>
       </c>
@@ -943,8 +1097,11 @@
       <c r="H13" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I13" s="3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>60</v>
       </c>
@@ -964,8 +1121,11 @@
       <c r="H14" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I14" s="3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -983,8 +1143,11 @@
       <c r="H15" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I15" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>62</v>
       </c>
@@ -1002,8 +1165,11 @@
       <c r="H16" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I16" s="3" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>41</v>
       </c>
@@ -1025,8 +1191,11 @@
       <c r="H17" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I17" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>63</v>
       </c>
@@ -1048,8 +1217,11 @@
       <c r="H18" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I18" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>64</v>
       </c>
@@ -1067,8 +1239,11 @@
       <c r="H19" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I19" s="3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>65</v>
       </c>
@@ -1094,8 +1269,11 @@
       <c r="H20" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I20" s="3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>66</v>
       </c>
@@ -1115,8 +1293,11 @@
       <c r="H21" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I21" s="3" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>67</v>
       </c>
@@ -1140,8 +1321,11 @@
       <c r="H22" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I22" s="3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>68</v>
       </c>
@@ -1159,8 +1343,11 @@
       <c r="H23" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I23" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>69</v>
       </c>
@@ -1186,8 +1373,11 @@
       <c r="H24" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I24" s="3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>1</v>
       </c>
@@ -1209,8 +1399,11 @@
       <c r="H25" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I25" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>7</v>
       </c>
@@ -1228,8 +1421,11 @@
       <c r="H26" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I26" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>8</v>
       </c>
@@ -1255,8 +1451,11 @@
       <c r="H27" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I27" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>11</v>
       </c>
@@ -1282,8 +1481,11 @@
       <c r="H28" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I28" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>70</v>
       </c>
@@ -1303,8 +1505,11 @@
       <c r="H29" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I29" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>71</v>
       </c>
@@ -1324,8 +1529,11 @@
       <c r="H30" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I30" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>72</v>
       </c>
@@ -1345,8 +1553,11 @@
       <c r="H31" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I31" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>73</v>
       </c>
@@ -1370,8 +1581,11 @@
       <c r="H32" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I32" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>61</v>
       </c>
@@ -1395,8 +1609,11 @@
       <c r="H33" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I33" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>44</v>
       </c>
@@ -1414,8 +1631,11 @@
       <c r="H34" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I34" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>45</v>
       </c>
@@ -1439,8 +1659,11 @@
       <c r="H35" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I35" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>48</v>
       </c>
@@ -1458,8 +1681,11 @@
       <c r="H36" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I36" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>49</v>
       </c>
@@ -1477,8 +1703,11 @@
       <c r="H37" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I37" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>50</v>
       </c>
@@ -1496,8 +1725,11 @@
       <c r="H38" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I38" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>51</v>
       </c>
@@ -1515,8 +1747,11 @@
       <c r="H39" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I39" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>52</v>
       </c>
@@ -1534,8 +1769,11 @@
       <c r="H40" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I40" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>53</v>
       </c>
@@ -1552,6 +1790,9 @@
       </c>
       <c r="H41" s="1" t="s">
         <v>6</v>
+      </c>
+      <c r="I41" s="3" t="s">
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -1570,10 +1811,10 @@
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -1691,7 +1932,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>